<commit_message>
Possibility to edit area from area list. Dynamic updating in area list when a new one is created
</commit_message>
<xml_diff>
--- a/fuelhunter_languages.xlsx
+++ b/fuelhunter_languages.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="664">
   <si>
     <t>COMMENT</t>
   </si>
@@ -1108,6 +1108,9 @@
     <t>degvielas uzpildes kompānijas</t>
   </si>
   <si>
+    <t>Rīga - 1 degvielas uzpildes kompānija</t>
+  </si>
+  <si>
     <t>areas_fuel_company</t>
   </si>
   <si>
@@ -1115,6 +1118,18 @@
   </si>
   <si>
     <t>degvielas uzpildes kompānija</t>
+  </si>
+  <si>
+    <t>Nav ieslēgta neviena degvielas uzpildes kompānijas</t>
+  </si>
+  <si>
+    <t>areas_fuel_company_empty_description</t>
+  </si>
+  <si>
+    <t>No fuel companies</t>
+  </si>
+  <si>
+    <t>Nav ieslēgta neviena degvielas uzpildes kompānija</t>
   </si>
   <si>
     <t>areas_name_title_description</t>
@@ -4044,328 +4059,328 @@
     </row>
     <row r="100">
       <c r="A100" s="4" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="4"/>
+      <c r="A101" s="4" t="s">
+        <v>369</v>
+      </c>
       <c r="B101" s="4" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="4"/>
       <c r="B102" s="4" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="4"/>
       <c r="B103" s="4" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="4"/>
       <c r="B104" s="4" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>162</v>
+        <v>381</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>162</v>
+        <v>381</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>162</v>
+        <v>381</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="4"/>
       <c r="B105" s="4" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>260</v>
+        <v>162</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>261</v>
+        <v>162</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>260</v>
+        <v>162</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="4"/>
       <c r="B106" s="4" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>187</v>
+        <v>385</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>188</v>
+        <v>260</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>189</v>
+        <v>261</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>188</v>
+        <v>260</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="4"/>
       <c r="B107" s="4" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>383</v>
+        <v>187</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>384</v>
+        <v>188</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>385</v>
+        <v>189</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>384</v>
+        <v>188</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="4"/>
       <c r="B108" s="4" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="E108" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="F108" s="4" t="s">
         <v>389</v>
-      </c>
-      <c r="F108" s="4" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="4"/>
       <c r="B109" s="4" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="4"/>
       <c r="B110" s="4" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="4"/>
       <c r="B111" s="4" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="4"/>
       <c r="B112" s="4" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="B113" s="3"/>
-      <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
-      <c r="E113" s="3"/>
-      <c r="F113" s="3"/>
+      <c r="A113" s="4"/>
+      <c r="B113" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="114">
-      <c r="A114" s="4" t="s">
-        <v>403</v>
-      </c>
-      <c r="B114" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="C114" s="4" t="s">
-        <v>405</v>
-      </c>
-      <c r="D114" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="E114" s="4" t="s">
+      <c r="A114" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="F114" s="4" t="s">
-        <v>406</v>
-      </c>
+      <c r="B114" s="3"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
+      <c r="E114" s="3"/>
+      <c r="F114" s="3"/>
     </row>
     <row r="115">
-      <c r="A115" s="5"/>
+      <c r="A115" s="4" t="s">
+        <v>408</v>
+      </c>
       <c r="B115" s="4" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E115" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="F115" s="4" t="s">
         <v>411</v>
-      </c>
-      <c r="F115" s="4" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="5"/>
       <c r="B116" s="4" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E116" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="F116" s="4" t="s">
         <v>415</v>
-      </c>
-      <c r="F116" s="4" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="5"/>
       <c r="B117" s="4" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E117" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="F117" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="F117" s="4" t="s">
-        <v>418</v>
-      </c>
     </row>
     <row r="118">
-      <c r="A118" s="4" t="s">
-        <v>420</v>
-      </c>
+      <c r="A118" s="5"/>
       <c r="B118" s="4" t="s">
         <v>421</v>
       </c>
@@ -4383,45 +4398,45 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="5"/>
+      <c r="A119" s="4" t="s">
+        <v>425</v>
+      </c>
       <c r="B119" s="4" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E119" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="F119" s="4" t="s">
         <v>428</v>
-      </c>
-      <c r="F119" s="4" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="5"/>
       <c r="B120" s="4" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E120" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="F120" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="F120" s="4" t="s">
-        <v>431</v>
-      </c>
     </row>
     <row r="121">
-      <c r="A121" s="4" t="s">
-        <v>433</v>
-      </c>
+      <c r="A121" s="5"/>
       <c r="B121" s="4" t="s">
         <v>434</v>
       </c>
@@ -4439,50 +4454,50 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="5"/>
+      <c r="A122" s="4" t="s">
+        <v>438</v>
+      </c>
       <c r="B122" s="4" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E122" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="F122" s="4" t="s">
         <v>441</v>
-      </c>
-      <c r="F122" s="4" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="5"/>
       <c r="B123" s="4" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E123" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="F123" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="F123" s="4" t="s">
-        <v>446</v>
-      </c>
     </row>
     <row r="124">
-      <c r="A124" s="4" t="s">
+      <c r="A124" s="5"/>
+      <c r="B124" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="C124" s="4" t="s">
         <v>448</v>
-      </c>
-      <c r="C124" s="4" t="s">
-        <v>449</v>
       </c>
       <c r="D124" s="4" t="s">
         <v>449</v>
@@ -4491,38 +4506,38 @@
         <v>450</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="4" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="E125" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="F125" s="4" t="s">
         <v>454</v>
-      </c>
-      <c r="F125" s="4" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="4" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D126" s="4" t="s">
         <v>458</v>
@@ -4555,1642 +4570,1654 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="5"/>
+      <c r="A128" s="4" t="s">
+        <v>465</v>
+      </c>
       <c r="B128" s="4" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="F128" s="4" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="5"/>
       <c r="B129" s="4" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="E129" s="4" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="F129" s="4" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="5"/>
       <c r="B130" s="4" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="F130" s="4" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="B131" s="3"/>
-      <c r="C131" s="3"/>
-      <c r="D131" s="3"/>
-      <c r="E131" s="3"/>
-      <c r="F131" s="3"/>
+      <c r="A131" s="5"/>
+      <c r="B131" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="D131" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="E131" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="F131" s="4" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="132">
-      <c r="A132" s="4" t="s">
-        <v>472</v>
-      </c>
-      <c r="B132" s="4" t="s">
-        <v>473</v>
-      </c>
-      <c r="C132" s="4" t="s">
+      <c r="A132" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="B132" s="3"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="3"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="C133" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="D132" s="4" t="s">
+      <c r="D133" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="E132" s="4" t="s">
+      <c r="E133" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="F132" s="4" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" s="5"/>
-      <c r="B133" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="C133" s="4" t="s">
+      <c r="F133" s="4" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="5"/>
+      <c r="B134" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="C134" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="D133" s="4" t="s">
+      <c r="D134" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E133" s="4" t="s">
+      <c r="E134" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="F133" s="4" t="s">
+      <c r="F134" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="134">
-      <c r="A134" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="B134" s="3"/>
-      <c r="C134" s="3"/>
-      <c r="D134" s="3"/>
-      <c r="E134" s="3"/>
-      <c r="F134" s="3"/>
-    </row>
     <row r="135">
-      <c r="A135" s="4" t="s">
-        <v>477</v>
-      </c>
-      <c r="B135" s="4" t="s">
-        <v>478</v>
-      </c>
-      <c r="C135" s="4" t="s">
+      <c r="A135" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B135" s="3"/>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
+      <c r="E135" s="3"/>
+      <c r="F135" s="3"/>
+    </row>
+    <row r="136">
+      <c r="A136" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="C136" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="D135" s="4" t="s">
+      <c r="D136" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="E135" s="4" t="s">
+      <c r="E136" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="F135" s="4" t="s">
+      <c r="F136" s="4" t="s">
         <v>326</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" s="5"/>
-      <c r="B136" s="4" t="s">
-        <v>479</v>
-      </c>
-      <c r="C136" s="4" t="s">
-        <v>480</v>
-      </c>
-      <c r="D136" s="4" t="s">
-        <v>481</v>
-      </c>
-      <c r="E136" s="4" t="s">
-        <v>482</v>
-      </c>
-      <c r="F136" s="4" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="5"/>
       <c r="B137" s="4" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="D137" s="4" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="E137" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="F137" s="4" t="s">
         <v>486</v>
-      </c>
-      <c r="F137" s="4" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="5"/>
       <c r="B138" s="4" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="D138" s="4" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E138" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="F138" s="4" t="s">
         <v>490</v>
-      </c>
-      <c r="F138" s="4" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="5"/>
       <c r="B139" s="4" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="E139" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="F139" s="4" t="s">
         <v>494</v>
-      </c>
-      <c r="F139" s="4" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="5"/>
       <c r="B140" s="4" t="s">
-        <v>495</v>
-      </c>
-      <c r="C140" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="D140" s="6" t="s">
+      <c r="C140" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="E140" s="6" t="s">
+      <c r="D140" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="F140" s="6" t="s">
-        <v>497</v>
+      <c r="E140" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="F140" s="4" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="B141" s="3"/>
-      <c r="C141" s="3"/>
-      <c r="D141" s="3"/>
-      <c r="E141" s="3"/>
-      <c r="F141" s="3"/>
+      <c r="A141" s="5"/>
+      <c r="B141" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="C141" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="D141" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="E141" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="F141" s="6" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="142">
-      <c r="A142" s="4" t="s">
-        <v>500</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>501</v>
-      </c>
-      <c r="C142" s="6" t="s">
-        <v>502</v>
-      </c>
-      <c r="D142" s="4" t="s">
-        <v>503</v>
-      </c>
-      <c r="E142" s="4" t="s">
+      <c r="A142" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="F142" s="4" t="s">
-        <v>503</v>
-      </c>
+      <c r="B142" s="3"/>
+      <c r="C142" s="3"/>
+      <c r="D142" s="3"/>
+      <c r="E142" s="3"/>
+      <c r="F142" s="3"/>
     </row>
     <row r="143">
-      <c r="A143" s="2" t="s">
+      <c r="A143" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="B143" s="3"/>
-      <c r="C143" s="3"/>
-      <c r="D143" s="3"/>
-      <c r="E143" s="3"/>
-      <c r="F143" s="3"/>
+      <c r="B143" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="C143" s="6" t="s">
+        <v>507</v>
+      </c>
+      <c r="D143" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="E143" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="F143" s="4" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="144">
-      <c r="A144" s="5"/>
-      <c r="B144" s="4" t="s">
-        <v>506</v>
-      </c>
-      <c r="C144" s="4" t="s">
-        <v>506</v>
-      </c>
-      <c r="D144" s="4" t="s">
-        <v>506</v>
-      </c>
-      <c r="E144" s="4" t="s">
-        <v>507</v>
-      </c>
-      <c r="F144" s="4" t="s">
-        <v>506</v>
-      </c>
+      <c r="A144" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="B144" s="3"/>
+      <c r="C144" s="3"/>
+      <c r="D144" s="3"/>
+      <c r="E144" s="3"/>
+      <c r="F144" s="3"/>
     </row>
     <row r="145">
       <c r="A145" s="5"/>
       <c r="B145" s="4" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="E145" s="4" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="F145" s="4" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="5"/>
       <c r="B146" s="4" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="D146" s="4" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="E146" s="4" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="F146" s="4" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="5"/>
       <c r="B147" s="4" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="D147" s="4" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="E147" s="4" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="F147" s="4" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="5"/>
       <c r="B148" s="4" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="E148" s="4" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="F148" s="4" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="5"/>
       <c r="B149" s="4" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="E149" s="4" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="F149" s="4" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="5"/>
       <c r="B150" s="4" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="E150" s="4" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="F150" s="4" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="5"/>
       <c r="B151" s="4" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="E151" s="4" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="F151" s="4" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="5"/>
       <c r="B152" s="4" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="E152" s="4" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="F152" s="4" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="5"/>
       <c r="B153" s="4" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="E153" s="4" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="F153" s="4" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="5"/>
       <c r="B154" s="4" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="E154" s="4" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="F154" s="4" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="5"/>
       <c r="B155" s="4" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="E155" s="4" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="F155" s="4" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="5"/>
       <c r="B156" s="4" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="D156" s="4" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="E156" s="4" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="F156" s="4" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="5"/>
       <c r="B157" s="4" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="E157" s="4" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="F157" s="4" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="5"/>
       <c r="B158" s="4" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="D158" s="4" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="F158" s="4" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="5"/>
       <c r="B159" s="4" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="F159" s="4" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="5"/>
       <c r="B160" s="4" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="F160" s="4" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="5"/>
       <c r="B161" s="4" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="F161" s="4" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="5"/>
       <c r="B162" s="4" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="D162" s="4" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="E162" s="4" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="F162" s="4" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="5"/>
       <c r="B163" s="4" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="F163" s="4" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="5"/>
       <c r="B164" s="4" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="E164" s="4" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="F164" s="4" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="5"/>
       <c r="B165" s="4" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="E165" s="4" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="F165" s="4" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="5"/>
       <c r="B166" s="4" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="E166" s="4" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="F166" s="4" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="5"/>
       <c r="B167" s="4" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="E167" s="4" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="F167" s="4" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="5"/>
       <c r="B168" s="4" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="E168" s="4" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="F168" s="4" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="5"/>
       <c r="B169" s="4" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="D169" s="4" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="E169" s="4" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="F169" s="4" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="5"/>
       <c r="B170" s="4" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="D170" s="4" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="E170" s="4" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="F170" s="4" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="5"/>
       <c r="B171" s="4" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="D171" s="4" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="E171" s="4" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="F171" s="4" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="5"/>
       <c r="B172" s="4" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="D172" s="4" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="E172" s="4" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="F172" s="4" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="5"/>
       <c r="B173" s="4" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="D173" s="4" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="E173" s="4" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="F173" s="4" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="5"/>
       <c r="B174" s="4" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="D174" s="4" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="E174" s="4" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="F174" s="4" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="5"/>
       <c r="B175" s="4" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="D175" s="4" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="E175" s="4" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="F175" s="4" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="5"/>
       <c r="B176" s="4" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="D176" s="4" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="E176" s="4" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="F176" s="4" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="5"/>
       <c r="B177" s="4" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="D177" s="4" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="E177" s="4" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="F177" s="4" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="5"/>
       <c r="B178" s="4" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="D178" s="4" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="E178" s="4" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="F178" s="4" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="5"/>
       <c r="B179" s="4" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="D179" s="4" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="E179" s="4" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="F179" s="4" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="5"/>
       <c r="B180" s="4" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="D180" s="4" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="E180" s="4" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="F180" s="4" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="5"/>
       <c r="B181" s="4" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="D181" s="4" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="E181" s="4" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="F181" s="4" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="5"/>
       <c r="B182" s="4" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="D182" s="4" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="E182" s="4" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="F182" s="4" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="5"/>
       <c r="B183" s="4" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="D183" s="4" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="E183" s="4" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="F183" s="4" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="5"/>
       <c r="B184" s="4" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="D184" s="4" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="E184" s="4" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="F184" s="4" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="5"/>
       <c r="B185" s="4" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="D185" s="4" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="E185" s="4" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="F185" s="4" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="5"/>
       <c r="B186" s="4" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="D186" s="4" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="E186" s="4" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="F186" s="4" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="5"/>
       <c r="B187" s="4" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="D187" s="4" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="E187" s="4" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="F187" s="4" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="5"/>
       <c r="B188" s="4" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="D188" s="4" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="E188" s="4" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="F188" s="4" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="5"/>
       <c r="B189" s="4" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="D189" s="4" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="E189" s="4" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="F189" s="4" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="5"/>
       <c r="B190" s="4" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="D190" s="4" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="E190" s="4" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="F190" s="4" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="5"/>
       <c r="B191" s="4" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="D191" s="4" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="E191" s="4" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="F191" s="4" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="5"/>
       <c r="B192" s="4" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="D192" s="4" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="E192" s="4" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="F192" s="4" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="5"/>
       <c r="B193" s="4" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="D193" s="4" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="E193" s="4" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="F193" s="4" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="5"/>
       <c r="B194" s="4" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="D194" s="4" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="E194" s="4" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="F194" s="4" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="5"/>
       <c r="B195" s="4" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="D195" s="4" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="E195" s="4" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="F195" s="4" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="5"/>
       <c r="B196" s="4" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="D196" s="4" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="E196" s="4" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="F196" s="4" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="5"/>
       <c r="B197" s="4" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="D197" s="4" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="E197" s="4" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="F197" s="4" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="5"/>
       <c r="B198" s="4" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="D198" s="4" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="E198" s="4" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="F198" s="4" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="5"/>
       <c r="B199" s="4" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="D199" s="4" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="E199" s="4" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="F199" s="4" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="5"/>
       <c r="B200" s="4" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="D200" s="4" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="E200" s="4" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="F200" s="4" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="5"/>
       <c r="B201" s="4" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="D201" s="4" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="E201" s="4" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="F201" s="4" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="5"/>
       <c r="B202" s="4" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="D202" s="4" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="E202" s="4" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="F202" s="4" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="5"/>
       <c r="B203" s="4" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="D203" s="4" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="E203" s="4" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="F203" s="4" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="5"/>
       <c r="B204" s="4" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="D204" s="4" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="E204" s="4" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="F204" s="4" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="5"/>
       <c r="B205" s="4" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="D205" s="4" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="E205" s="4" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="F205" s="4" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="5"/>
       <c r="B206" s="4" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="D206" s="4" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="E206" s="4" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="F206" s="4" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="5"/>
       <c r="B207" s="4" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="D207" s="4" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="E207" s="4" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="F207" s="4" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="5"/>
       <c r="B208" s="4" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="D208" s="4" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="E208" s="4" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="F208" s="4" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="5"/>
       <c r="B209" s="4" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="D209" s="4" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="E209" s="4" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="F209" s="4" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="5"/>
       <c r="B210" s="4" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="D210" s="4" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="E210" s="4" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="F210" s="4" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="5"/>
       <c r="B211" s="4" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="D211" s="4" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="E211" s="4" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="F211" s="4" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="5"/>
       <c r="B212" s="4" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="D212" s="4" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="E212" s="4" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="F212" s="4" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="5"/>
       <c r="B213" s="4" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="D213" s="4" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="E213" s="4" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="F213" s="4" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="5"/>
       <c r="B214" s="4" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="D214" s="4" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="E214" s="4" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="F214" s="4" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="5"/>
       <c r="B215" s="4" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="D215" s="4" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="E215" s="4" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="F215" s="4" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="5"/>
       <c r="B216" s="4" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="D216" s="4" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="E216" s="4" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="F216" s="4" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="5"/>
       <c r="B217" s="4" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="D217" s="4" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="E217" s="4" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="F217" s="4" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="5"/>
       <c r="B218" s="4" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="D218" s="4" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="E218" s="4" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="F218" s="4" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="5"/>
       <c r="B219" s="4" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="D219" s="4" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="E219" s="4" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="F219" s="4" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="220">
-      <c r="A220" s="8"/>
-      <c r="B220" s="8"/>
-      <c r="C220" s="8"/>
-      <c r="D220" s="8"/>
-      <c r="E220" s="8"/>
-      <c r="F220" s="8"/>
+      <c r="A220" s="5"/>
+      <c r="B220" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="C220" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="D220" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="E220" s="4" t="s">
+        <v>663</v>
+      </c>
+      <c r="F220" s="4" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="8"/>
@@ -6346,7 +6373,7 @@
     </row>
     <row r="240">
       <c r="A240" s="8"/>
-      <c r="B240" s="9"/>
+      <c r="B240" s="8"/>
       <c r="C240" s="8"/>
       <c r="D240" s="8"/>
       <c r="E240" s="8"/>
@@ -6944,6 +6971,14 @@
       <c r="E314" s="8"/>
       <c r="F314" s="8"/>
     </row>
+    <row r="315">
+      <c r="A315" s="8"/>
+      <c r="B315" s="9"/>
+      <c r="C315" s="8"/>
+      <c r="D315" s="8"/>
+      <c r="E315" s="8"/>
+      <c r="F315" s="8"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>